<commit_message>
Mobile script and output files
Small easing same as moderate easing issue
</commit_message>
<xml_diff>
--- a/data/input_data_US_mobile.xlsx
+++ b/data/input_data_US_mobile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sherr\Documents\GitHub\covasim-australia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D08E896-BE5B-4831-A91F-03DA1672C428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98346069-AE11-4D88-A911-E019CA42831A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="815" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="10420" tabRatio="815" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age_sex" sheetId="1" r:id="rId1"/>
@@ -130,6 +130,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={E28F53A2-63DB-45F9-A493-D37922578F96}</author>
+    <author>tc={099054D7-036B-4D24-B641-708A03048C6C}</author>
+    <author>tc={EC86CD57-281C-41CF-9A03-13B393CCD846}</author>
   </authors>
   <commentList>
     <comment ref="C9" authorId="0" shapeId="0" xr:uid="{E28F53A2-63DB-45F9-A493-D37922578F96}">
@@ -138,6 +140,22 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Hypothetical: remove start date (no end date needed)</t>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="1" shapeId="0" xr:uid="{099054D7-036B-4D24-B641-708A03048C6C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Standard increase: absolute increase of 10% over latest policy</t>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="2" shapeId="0" xr:uid="{EC86CD57-281C-41CF-9A03-13B393CCD846}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Standard increase: absolute increase of 20% over latest policy</t>
       </text>
     </comment>
   </commentList>
@@ -462,10 +480,10 @@
     <t>relax5</t>
   </si>
   <si>
-    <t>Onside food/drink service in restaurants, bars, breweries prohibited; Public schools closed; Gatherings 25+ restricted, hospital, care home, LTC visitation prohibited</t>
-  </si>
-  <si>
     <t>from 1.5</t>
+  </si>
+  <si>
+    <t>Onsite food/drink service in restaurants, bars, breweries prohibited; Public schools closed; Gatherings 25+ restricted, hospital, care home, LTC visitation prohibited</t>
   </si>
 </sst>
 </file>
@@ -476,7 +494,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -563,6 +581,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1023,6 +1047,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1040,12 +1070,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1410,6 +1434,12 @@
   <threadedComment ref="C9" dT="2020-08-02T23:54:02.44" personId="{500D21BA-0542-41FF-BB3D-9ABDB93A6223}" id="{E28F53A2-63DB-45F9-A493-D37922578F96}">
     <text>Hypothetical: remove start date (no end date needed)</text>
   </threadedComment>
+  <threadedComment ref="D9" dT="2020-08-06T02:31:10.85" personId="{500D21BA-0542-41FF-BB3D-9ABDB93A6223}" id="{099054D7-036B-4D24-B641-708A03048C6C}">
+    <text>Standard increase: absolute increase of 10% over latest policy</text>
+  </threadedComment>
+  <threadedComment ref="D10" dT="2020-08-06T02:31:16.42" personId="{500D21BA-0542-41FF-BB3D-9ABDB93A6223}" id="{EC86CD57-281C-41CF-9A03-13B393CCD846}">
+    <text>Standard increase: absolute increase of 20% over latest policy</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1501,7 +1531,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="70" t="s">
         <v>88</v>
       </c>
       <c r="B2" s="26" t="s">
@@ -1561,7 +1591,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A3" s="68"/>
+      <c r="A3" s="70"/>
       <c r="B3" s="26" t="s">
         <v>20</v>
       </c>
@@ -1619,7 +1649,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="70" t="s">
         <v>88</v>
       </c>
       <c r="B4" s="26" t="s">
@@ -1695,7 +1725,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" s="68"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="26" t="s">
         <v>21</v>
       </c>
@@ -1934,7 +1964,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="74" t="s">
         <v>88</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -1993,7 +2023,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="72"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
@@ -2050,7 +2080,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="72"/>
+      <c r="A4" s="74"/>
       <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
@@ -2107,7 +2137,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="72"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
@@ -2164,7 +2194,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="72"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
@@ -2221,7 +2251,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="72"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="15" t="s">
         <v>5</v>
       </c>
@@ -2278,7 +2308,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="72"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
@@ -2335,7 +2365,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="72"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
@@ -2392,7 +2422,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="72"/>
+      <c r="A10" s="74"/>
       <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
@@ -2449,7 +2479,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="72"/>
+      <c r="A11" s="74"/>
       <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
@@ -2506,7 +2536,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="72"/>
+      <c r="A12" s="74"/>
       <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
@@ -2563,7 +2593,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="72"/>
+      <c r="A13" s="74"/>
       <c r="B13" s="15" t="s">
         <v>11</v>
       </c>
@@ -2620,7 +2650,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="72"/>
+      <c r="A14" s="74"/>
       <c r="B14" s="15" t="s">
         <v>12</v>
       </c>
@@ -2677,7 +2707,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="72"/>
+      <c r="A15" s="74"/>
       <c r="B15" s="15" t="s">
         <v>13</v>
       </c>
@@ -2734,7 +2764,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="72"/>
+      <c r="A16" s="74"/>
       <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
@@ -2791,7 +2821,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="72"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="15" t="s">
         <v>15</v>
       </c>
@@ -2933,7 +2963,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="74" t="s">
         <v>88</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -2992,7 +3022,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="72"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
@@ -3049,7 +3079,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="72"/>
+      <c r="A4" s="74"/>
       <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
@@ -3106,7 +3136,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="72"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
@@ -3163,7 +3193,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="72"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
@@ -3220,7 +3250,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="72"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="15" t="s">
         <v>5</v>
       </c>
@@ -3277,7 +3307,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="72"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
@@ -3334,7 +3364,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="72"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
@@ -3391,7 +3421,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="72"/>
+      <c r="A10" s="74"/>
       <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
@@ -3448,7 +3478,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="72"/>
+      <c r="A11" s="74"/>
       <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
@@ -3505,7 +3535,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="72"/>
+      <c r="A12" s="74"/>
       <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
@@ -3562,7 +3592,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="72"/>
+      <c r="A13" s="74"/>
       <c r="B13" s="15" t="s">
         <v>11</v>
       </c>
@@ -3619,7 +3649,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="72"/>
+      <c r="A14" s="74"/>
       <c r="B14" s="15" t="s">
         <v>12</v>
       </c>
@@ -3676,7 +3706,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="72"/>
+      <c r="A15" s="74"/>
       <c r="B15" s="15" t="s">
         <v>13</v>
       </c>
@@ -3733,7 +3763,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="72"/>
+      <c r="A16" s="74"/>
       <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
@@ -3790,7 +3820,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="72"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="15" t="s">
         <v>15</v>
       </c>
@@ -3927,7 +3957,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="75" t="s">
         <v>88</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -3986,7 +4016,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="73"/>
+      <c r="A3" s="75"/>
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
@@ -4043,7 +4073,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="73"/>
+      <c r="A4" s="75"/>
       <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
@@ -4100,7 +4130,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="73"/>
+      <c r="A5" s="75"/>
       <c r="B5" s="13" t="s">
         <v>3</v>
       </c>
@@ -4157,7 +4187,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="73"/>
+      <c r="A6" s="75"/>
       <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
@@ -4214,7 +4244,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="73"/>
+      <c r="A7" s="75"/>
       <c r="B7" s="13" t="s">
         <v>5</v>
       </c>
@@ -4271,7 +4301,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="73"/>
+      <c r="A8" s="75"/>
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
@@ -4328,7 +4358,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="73"/>
+      <c r="A9" s="75"/>
       <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
@@ -4385,7 +4415,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="73"/>
+      <c r="A10" s="75"/>
       <c r="B10" s="13" t="s">
         <v>8</v>
       </c>
@@ -4442,7 +4472,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="73"/>
+      <c r="A11" s="75"/>
       <c r="B11" s="13" t="s">
         <v>9</v>
       </c>
@@ -4499,7 +4529,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="73"/>
+      <c r="A12" s="75"/>
       <c r="B12" s="13" t="s">
         <v>10</v>
       </c>
@@ -4556,7 +4586,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="73"/>
+      <c r="A13" s="75"/>
       <c r="B13" s="13" t="s">
         <v>11</v>
       </c>
@@ -4613,7 +4643,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="73"/>
+      <c r="A14" s="75"/>
       <c r="B14" s="13" t="s">
         <v>12</v>
       </c>
@@ -4670,7 +4700,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="73"/>
+      <c r="A15" s="75"/>
       <c r="B15" s="13" t="s">
         <v>13</v>
       </c>
@@ -4727,7 +4757,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="73"/>
+      <c r="A16" s="75"/>
       <c r="B16" s="13" t="s">
         <v>14</v>
       </c>
@@ -4784,7 +4814,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="73"/>
+      <c r="A17" s="75"/>
       <c r="B17" s="13" t="s">
         <v>15</v>
       </c>
@@ -5413,10 +5443,10 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R25" sqref="R25"/>
-      <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5473,7 +5503,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="71" t="s">
         <v>88</v>
       </c>
       <c r="B2" s="47" t="s">
@@ -5510,12 +5540,12 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="70"/>
+      <c r="A3" s="72"/>
       <c r="B3" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D3" s="58">
         <v>0.89</v>
@@ -5546,7 +5576,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="70"/>
+      <c r="A4" s="72"/>
       <c r="B4" s="35" t="s">
         <v>70</v>
       </c>
@@ -5582,7 +5612,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="35" t="s">
         <v>84</v>
       </c>
@@ -5618,7 +5648,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="70"/>
+      <c r="A6" s="72"/>
       <c r="B6" s="35" t="s">
         <v>71</v>
       </c>
@@ -5654,7 +5684,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="70"/>
+      <c r="A7" s="72"/>
       <c r="B7" s="35" t="s">
         <v>72</v>
       </c>
@@ -5690,7 +5720,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="70"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="35" t="s">
         <v>73</v>
       </c>
@@ -5723,16 +5753,16 @@
       <c r="M8" s="65"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="70"/>
+      <c r="A9" s="72"/>
       <c r="B9" s="35" t="s">
         <v>92</v>
       </c>
       <c r="C9" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="74">
-        <f>(D8*0.1)+D8</f>
-        <v>0.42900000000000005</v>
+      <c r="D9" s="68">
+        <f>D8+0.3</f>
+        <v>0.69</v>
       </c>
       <c r="E9" s="35">
         <v>1</v>
@@ -5755,16 +5785,16 @@
       <c r="M9" s="66"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="71"/>
+      <c r="A10" s="73"/>
       <c r="B10" s="44" t="s">
         <v>95</v>
       </c>
       <c r="C10" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="75">
-        <f>(D8*0.2)+D8</f>
-        <v>0.46800000000000003</v>
+      <c r="D10" s="69">
+        <f>D8+0.6</f>
+        <v>0.99</v>
       </c>
       <c r="E10" s="44">
         <v>1</v>
@@ -5985,7 +6015,7 @@
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="Q3" s="63"/>
       <c r="S3" s="52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update input databook Mobile
</commit_message>
<xml_diff>
--- a/data/input_data_US_mobile.xlsx
+++ b/data/input_data_US_mobile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sherr\Documents\GitHub\covasim-australia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98346069-AE11-4D88-A911-E019CA42831A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FDE7C9-0D05-4418-90B4-152291138A93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="10420" tabRatio="815" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1070" yWindow="1060" windowWidth="15360" windowHeight="7360" tabRatio="815" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age_sex" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -581,12 +581,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -5446,14 +5440,14 @@
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R25" sqref="R25"/>
-      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
+      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.6328125" style="22" customWidth="1"/>
     <col min="2" max="2" width="10.36328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.36328125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="25.54296875" style="22" customWidth="1"/>
     <col min="4" max="4" width="6.90625" style="24" customWidth="1"/>
     <col min="5" max="11" width="1.6328125" style="22" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="16.453125" style="22" customWidth="1"/>

</xml_diff>

<commit_message>
Mobile and Rotterdam files
</commit_message>
<xml_diff>
--- a/data/input_data_US_mobile.xlsx
+++ b/data/input_data_US_mobile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farah.houdroge\Documents\GitHub\covasim-australia\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sherr\Documents\GitHub\covasim-australia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAFB62B-5F3B-4CB7-906D-FA0CA657C3F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44A0000-D2A5-4ECD-A33E-338D9ED8FE62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="815" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="815" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age_sex" sheetId="1" r:id="rId1"/>
@@ -450,30 +450,15 @@
     <t>State of emergency declared</t>
   </si>
   <si>
-    <t>Compulsory mask wearing</t>
-  </si>
-  <si>
     <t>Hypothetical relaxation</t>
   </si>
   <si>
     <t>Mobile</t>
   </si>
   <si>
-    <t>Stay-at-home order</t>
-  </si>
-  <si>
-    <t>Safer-at-Home order (some reopenings)</t>
-  </si>
-  <si>
-    <t>Safer-at-Home order relaxed (childcare, camps, retailers, athletic facilities, theaters reopened)</t>
-  </si>
-  <si>
     <t>relax4</t>
   </si>
   <si>
-    <t>Gathering 10+ restricted, all schools closed, non-emergency dental/surgeries suspended</t>
-  </si>
-  <si>
     <t>Contact tracing via health department phone calls</t>
   </si>
   <si>
@@ -483,7 +468,22 @@
     <t>from 1.5</t>
   </si>
   <si>
-    <t>Onsite food/drink service in restaurants, bars, breweries prohibited; Public schools closed; Gatherings 25+ restricted, hospital, care home, LTC visitation prohibited</t>
+    <t>Mandatory mask order issued</t>
+  </si>
+  <si>
+    <t>Stay at home order issued</t>
+  </si>
+  <si>
+    <t>Gatherings limited to 25 people, public schools closed, healthcare center visitation prohibited, and hospitality limited</t>
+  </si>
+  <si>
+    <t>Gatherings limited to 10 people, all schools closed, and non-emergency health services suspended</t>
+  </si>
+  <si>
+    <t>Some reopenings</t>
+  </si>
+  <si>
+    <t>Childcare, summer camps, retailers, athletic centers, and theaters reopened</t>
   </si>
 </sst>
 </file>
@@ -493,9 +493,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,6 +579,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -873,7 +880,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1033,6 +1040,27 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1051,27 +1079,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1463,16 +1471,16 @@
       <selection activeCell="C2" sqref="C2:S5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="18" width="6.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="27"/>
+    <col min="3" max="18" width="6.453125" style="27" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.453125" style="27" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -1531,9 +1539,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
-        <v>88</v>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" s="72" t="s">
+        <v>87</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>19</v>
@@ -1591,8 +1599,8 @@
         <v>207389</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="72"/>
       <c r="B3" s="26" t="s">
         <v>20</v>
       </c>
@@ -1649,9 +1657,9 @@
         <v>192944</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
-        <v>88</v>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="72" t="s">
+        <v>87</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>16</v>
@@ -1725,8 +1733,8 @@
         <v>400333</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="65"/>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="72"/>
       <c r="B5" s="26" t="s">
         <v>21</v>
       </c>
@@ -1798,82 +1806,82 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C6" s="28"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C7" s="28"/>
       <c r="S7" s="37"/>
       <c r="T7" s="29"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C8" s="28"/>
       <c r="T8" s="29"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C9" s="28"/>
       <c r="T9" s="29"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
       <c r="T10" s="29"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
       <c r="D22" s="28"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
       <c r="D23" s="28"/>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
       <c r="D24" s="28"/>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
       <c r="D25" s="28"/>
     </row>
   </sheetData>
@@ -1900,12 +1908,12 @@
       <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="16"/>
+    <col min="1" max="16384" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>17</v>
       </c>
@@ -1964,9 +1972,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
-        <v>88</v>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="76" t="s">
+        <v>87</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>0</v>
@@ -2023,8 +2031,8 @@
         <v>3.5668052131556029</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="76"/>
       <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
@@ -2080,8 +2088,8 @@
         <v>4.0529896903791238</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="69"/>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="76"/>
       <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
@@ -2137,8 +2145,8 @@
         <v>4.3115733563210163</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="69"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="76"/>
       <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
@@ -2194,8 +2202,8 @@
         <v>3.629724341565661</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="69"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="76"/>
       <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
@@ -2251,8 +2259,8 @@
         <v>2.949193529531942</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="69"/>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="76"/>
       <c r="B7" s="15" t="s">
         <v>5</v>
       </c>
@@ -2308,8 +2316,8 @@
         <v>2.5959713809084199</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="69"/>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="76"/>
       <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
@@ -2365,8 +2373,8 @@
         <v>2.930654020980263</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="69"/>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="76"/>
       <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
@@ -2422,8 +2430,8 @@
         <v>3.462886762272865</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="69"/>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="76"/>
       <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
@@ -2479,8 +2487,8 @@
         <v>3.1796263978546309</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="69"/>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="76"/>
       <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
@@ -2536,8 +2544,8 @@
         <v>3.1822678358086711</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="69"/>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="76"/>
       <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
@@ -2593,8 +2601,8 @@
         <v>3.07658862942833</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="69"/>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="76"/>
       <c r="B13" s="15" t="s">
         <v>11</v>
       </c>
@@ -2650,8 +2658,8 @@
         <v>3.5861552161648351</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="69"/>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="76"/>
       <c r="B14" s="15" t="s">
         <v>12</v>
       </c>
@@ -2707,8 +2715,8 @@
         <v>3.001371404115428</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="69"/>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="76"/>
       <c r="B15" s="15" t="s">
         <v>13</v>
       </c>
@@ -2764,8 +2772,8 @@
         <v>2.9768279935895898</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="69"/>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="76"/>
       <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
@@ -2821,8 +2829,8 @@
         <v>2.4423431400467339</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="69"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="76"/>
       <c r="B17" s="15" t="s">
         <v>15</v>
       </c>
@@ -2899,12 +2907,12 @@
       <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="16"/>
+    <col min="1" max="16384" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>17</v>
       </c>
@@ -2963,9 +2971,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
-        <v>88</v>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="76" t="s">
+        <v>87</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>0</v>
@@ -3022,8 +3030,8 @@
         <v>1.9303406046028391</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="76"/>
       <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
@@ -3079,8 +3087,8 @@
         <v>3.7477763404398901</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="69"/>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="76"/>
       <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
@@ -3136,8 +3144,8 @@
         <v>5.4372924116155366</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="69"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="76"/>
       <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
@@ -3193,8 +3201,8 @@
         <v>7.7911518064499461</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="69"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="76"/>
       <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
@@ -3250,8 +3258,8 @@
         <v>1.141416962812404</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="69"/>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="76"/>
       <c r="B7" s="15" t="s">
         <v>5</v>
       </c>
@@ -3307,8 +3315,8 @@
         <v>0.74299743745883251</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="69"/>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="76"/>
       <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
@@ -3364,8 +3372,8 @@
         <v>0.91562964911041378</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="69"/>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="76"/>
       <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
@@ -3421,8 +3429,8 @@
         <v>0.6753458306423481</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="69"/>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="76"/>
       <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
@@ -3478,8 +3486,8 @@
         <v>0.76489167529992985</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="69"/>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="76"/>
       <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
@@ -3535,8 +3543,8 @@
         <v>1.453299615717849</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="69"/>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="76"/>
       <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
@@ -3592,8 +3600,8 @@
         <v>1.8367487786824079</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="69"/>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="76"/>
       <c r="B13" s="15" t="s">
         <v>11</v>
       </c>
@@ -3649,8 +3657,8 @@
         <v>1.562940460840295</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="69"/>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="76"/>
       <c r="B14" s="15" t="s">
         <v>12</v>
       </c>
@@ -3706,8 +3714,8 @@
         <v>0.57118490850485704</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="69"/>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="76"/>
       <c r="B15" s="15" t="s">
         <v>13</v>
       </c>
@@ -3763,8 +3771,8 @@
         <v>0.13510911184621879</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="69"/>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="76"/>
       <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
@@ -3820,8 +3828,8 @@
         <v>0.14601050001903429</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="69"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="76"/>
       <c r="B17" s="15" t="s">
         <v>15</v>
       </c>
@@ -3896,9 +3904,9 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
@@ -3957,9 +3965,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
-        <v>88</v>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="77" t="s">
+        <v>87</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>0</v>
@@ -4016,8 +4024,8 @@
         <v>1.2058515015357481E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="77"/>
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
@@ -4073,8 +4081,8 @@
         <v>1.3495557764948161E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="70"/>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="77"/>
       <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
@@ -4130,8 +4138,8 @@
         <v>0.2813185441721629</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="70"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="77"/>
       <c r="B5" s="13" t="s">
         <v>3</v>
       </c>
@@ -4187,8 +4195,8 @@
         <v>2.8842754143599101</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="70"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="77"/>
       <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
@@ -4244,8 +4252,8 @@
         <v>4.6393921641713387</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="70"/>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="77"/>
       <c r="B7" s="13" t="s">
         <v>5</v>
       </c>
@@ -4301,8 +4309,8 @@
         <v>6.1400745552879066</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="70"/>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="77"/>
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
@@ -4358,8 +4366,8 @@
         <v>5.8764005129956374</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="70"/>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="77"/>
       <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
@@ -4415,8 +4423,8 @@
         <v>6.3000370430396302</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="70"/>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="77"/>
       <c r="B10" s="13" t="s">
         <v>8</v>
       </c>
@@ -4472,8 +4480,8 @@
         <v>6.5027859240419721</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="70"/>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="77"/>
       <c r="B11" s="13" t="s">
         <v>9</v>
       </c>
@@ -4529,8 +4537,8 @@
         <v>5.3296444077456453</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="70"/>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="77"/>
       <c r="B12" s="13" t="s">
         <v>10</v>
       </c>
@@ -4586,8 +4594,8 @@
         <v>5.5825541518369617</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="70"/>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="77"/>
       <c r="B13" s="13" t="s">
         <v>11</v>
       </c>
@@ -4643,8 +4651,8 @@
         <v>3.6317270633078929</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="70"/>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="77"/>
       <c r="B14" s="13" t="s">
         <v>12</v>
       </c>
@@ -4700,8 +4708,8 @@
         <v>1.0832747747492379</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="70"/>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="77"/>
       <c r="B15" s="13" t="s">
         <v>13</v>
       </c>
@@ -4757,8 +4765,8 @@
         <v>6.0687793070067367E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="70"/>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="77"/>
       <c r="B16" s="13" t="s">
         <v>14</v>
       </c>
@@ -4814,8 +4822,8 @@
         <v>3.612164506622016E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="70"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="77"/>
       <c r="B17" s="13" t="s">
         <v>15</v>
       </c>
@@ -4887,14 +4895,14 @@
       <selection activeCell="B2" sqref="B2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="11.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="22"/>
+    <col min="1" max="2" width="8.1796875" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="11.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.81640625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>17</v>
       </c>
@@ -4917,9 +4925,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="38">
         <v>31.1</v>
@@ -4942,22 +4950,22 @@
       <c r="H2" s="38"/>
       <c r="I2" s="39"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" s="38"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" s="38"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" s="38"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="38"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" s="38"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="38"/>
     </row>
   </sheetData>
@@ -4975,22 +4983,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="27"/>
+    <col min="6" max="6" width="6.453125" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1796875" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="31" t="s">
         <v>17</v>
       </c>
@@ -5022,9 +5030,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="34">
         <v>3</v>
@@ -5069,22 +5077,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="27"/>
+    <col min="6" max="6" width="6.453125" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1796875" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.453125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="31" t="s">
         <v>17</v>
       </c>
@@ -5116,9 +5124,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="34">
         <v>4</v>
@@ -5162,21 +5170,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="3"/>
-    <col min="9" max="9" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" style="3"/>
+    <col min="9" max="9" width="10.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>17</v>
       </c>
@@ -5208,9 +5216,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="34">
         <v>18</v>
@@ -5240,7 +5248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B3" s="34"/>
       <c r="C3" s="35"/>
       <c r="D3" s="35"/>
@@ -5267,22 +5275,22 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="27"/>
+    <col min="6" max="6" width="6.453125" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1796875" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.453125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="31" t="s">
         <v>17</v>
       </c>
@@ -5314,9 +5322,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="34">
         <v>3</v>
@@ -5362,20 +5370,20 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
@@ -5404,15 +5412,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="45" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D2" s="46" t="s">
         <v>80</v>
@@ -5443,24 +5451,24 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R25" sqref="R25"/>
-      <selection pane="bottomLeft" activeCell="N20" sqref="N20"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="24" customWidth="1"/>
-    <col min="5" max="11" width="1.5703125" style="22" hidden="1" customWidth="1"/>
-    <col min="12" max="13" width="18.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="22"/>
+    <col min="1" max="1" width="6.54296875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" style="22" customWidth="1"/>
+    <col min="4" max="4" width="6.81640625" style="24" customWidth="1"/>
+    <col min="5" max="11" width="1.54296875" style="22" hidden="1" customWidth="1"/>
+    <col min="12" max="13" width="18.453125" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.81640625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>17</v>
       </c>
@@ -5501,9 +5509,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
-        <v>88</v>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="73" t="s">
+        <v>87</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>68</v>
@@ -5531,20 +5539,20 @@
       </c>
       <c r="J2" s="47"/>
       <c r="K2" s="47"/>
-      <c r="L2" s="75">
+      <c r="L2" s="69">
         <v>43903</v>
       </c>
-      <c r="M2" s="76">
+      <c r="M2" s="70">
         <v>43907</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="67"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="74"/>
       <c r="B3" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D3" s="56">
         <v>0.89</v>
@@ -5566,21 +5574,21 @@
       </c>
       <c r="J3" s="35"/>
       <c r="K3" s="35"/>
-      <c r="L3" s="77">
+      <c r="L3" s="71">
         <v>43907</v>
       </c>
-      <c r="M3" s="76">
+      <c r="M3" s="70">
         <f>L4</f>
         <v>43917</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="67"/>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="74"/>
       <c r="B4" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D4" s="56">
         <v>0.87</v>
@@ -5602,21 +5610,21 @@
       </c>
       <c r="J4" s="35"/>
       <c r="K4" s="35"/>
-      <c r="L4" s="77">
+      <c r="L4" s="71">
         <v>43917</v>
       </c>
-      <c r="M4" s="76">
+      <c r="M4" s="70">
         <f>L5</f>
         <v>43925</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="67"/>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="74"/>
       <c r="B5" s="35" t="s">
         <v>84</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D5" s="56">
         <v>0.35</v>
@@ -5638,21 +5646,21 @@
       </c>
       <c r="J5" s="35"/>
       <c r="K5" s="35"/>
-      <c r="L5" s="77">
+      <c r="L5" s="71">
         <v>43925</v>
       </c>
-      <c r="M5" s="76">
+      <c r="M5" s="70">
         <f>L6</f>
         <v>43951</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="74"/>
       <c r="B6" s="35" t="s">
         <v>71</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D6" s="56">
         <v>0.39</v>
@@ -5674,21 +5682,21 @@
       </c>
       <c r="J6" s="35"/>
       <c r="K6" s="35"/>
-      <c r="L6" s="77">
+      <c r="L6" s="71">
         <v>43951</v>
       </c>
-      <c r="M6" s="76">
+      <c r="M6" s="70">
         <f>L7</f>
         <v>43973</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="67"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="74"/>
       <c r="B7" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="48" t="s">
-        <v>91</v>
+      <c r="C7" s="78" t="s">
+        <v>97</v>
       </c>
       <c r="D7" s="56">
         <v>0.41</v>
@@ -5710,21 +5718,21 @@
       </c>
       <c r="J7" s="35"/>
       <c r="K7" s="35"/>
-      <c r="L7" s="77">
+      <c r="L7" s="71">
         <v>43973</v>
       </c>
-      <c r="M7" s="76">
+      <c r="M7" s="70">
         <f>L8</f>
         <v>44027</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="67"/>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="74"/>
       <c r="B8" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="35" t="s">
-        <v>86</v>
+      <c r="C8" s="78" t="s">
+        <v>92</v>
       </c>
       <c r="D8" s="56">
         <v>0.39</v>
@@ -5746,22 +5754,22 @@
       </c>
       <c r="J8" s="35"/>
       <c r="K8" s="35"/>
-      <c r="L8" s="77">
+      <c r="L8" s="71">
         <v>44027</v>
       </c>
-      <c r="M8" s="76"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="67"/>
+      <c r="M8" s="70"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="74"/>
       <c r="B9" s="35" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="63">
-        <f>D8+0.3</f>
-        <v>0.69</v>
+        <f>D8+0.1</f>
+        <v>0.49</v>
       </c>
       <c r="E9" s="35">
         <v>1</v>
@@ -5780,20 +5788,20 @@
       </c>
       <c r="J9" s="35"/>
       <c r="K9" s="35"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="71"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="68"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="65"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="75"/>
       <c r="B10" s="44" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="64">
-        <f>D8+0.6</f>
-        <v>0.99</v>
+        <f>D8+0.2</f>
+        <v>0.59000000000000008</v>
       </c>
       <c r="E10" s="44">
         <v>1</v>
@@ -5812,10 +5820,10 @@
       </c>
       <c r="J10" s="44"/>
       <c r="K10" s="44"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="74"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L10" s="67"/>
+      <c r="M10" s="68"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C12" s="60"/>
     </row>
   </sheetData>
@@ -5840,34 +5848,34 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.1796875" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.81640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" style="50" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" style="50" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.81640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" style="50" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" style="50" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.81640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" style="50" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" style="50" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" style="50" customWidth="1"/>
-    <col min="16" max="16" width="6.5703125" style="50" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" style="50" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.81640625" style="50" customWidth="1"/>
+    <col min="16" max="16" width="6.54296875" style="50" customWidth="1"/>
+    <col min="17" max="17" width="16.1796875" style="50" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.54296875" style="50" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" style="50" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.85546875" style="50"/>
+    <col min="21" max="21" width="9.453125" style="50" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.54296875" style="50" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.1796875" style="50" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.81640625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
         <v>17</v>
       </c>
@@ -5938,9 +5946,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="58">
         <v>43898</v>
@@ -6011,10 +6019,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="Q3" s="61"/>
       <c r="S3" s="50" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>